<commit_message>
Edit the files for the right normalization
</commit_message>
<xml_diff>
--- a/11_18_DCAA_Combo.xlsx
+++ b/11_18_DCAA_Combo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="124">
   <si>
     <t>Block Type</t>
   </si>
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD89"/>
+  <dimension ref="A1:AD92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3368,13 +3368,13 @@
         <v>47</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>0.78846567869186401</v>
       </c>
       <c r="H36">
-        <v>0.46823376417160034</v>
+        <v>0.36918628215789795</v>
       </c>
       <c r="I36">
-        <v>2.1356854438781738</v>
+        <v>1.6839146614074707</v>
       </c>
       <c r="J36">
         <v>29.451627731323242</v>
@@ -3401,7 +3401,7 @@
         <v>11</v>
       </c>
       <c r="R36">
-        <v>0</v>
+        <v>0.34288010001182556</v>
       </c>
       <c r="S36" t="b">
         <v>1</v>
@@ -3437,7 +3437,7 @@
         <v>49</v>
       </c>
       <c r="AD36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
@@ -3460,13 +3460,13 @@
         <v>47</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>0.78846567869186401</v>
       </c>
       <c r="H37">
-        <v>0.46823376417160034</v>
+        <v>0.36918628215789795</v>
       </c>
       <c r="I37">
-        <v>2.1356854438781738</v>
+        <v>1.6839146614074707</v>
       </c>
       <c r="J37">
         <v>27.944446563720703</v>
@@ -3493,7 +3493,7 @@
         <v>11</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>0.34288010001182556</v>
       </c>
       <c r="S37" t="b">
         <v>1</v>
@@ -3552,13 +3552,13 @@
         <v>47</v>
       </c>
       <c r="G38">
-        <v>2.354658842086792</v>
+        <v>1.8565676212310791</v>
       </c>
       <c r="H38">
-        <v>2.1266369819641113</v>
+        <v>1.6767802238464355</v>
       </c>
       <c r="I38">
-        <v>2.6071295738220215</v>
+        <v>2.0556321144104004</v>
       </c>
       <c r="J38">
         <v>26.855991363525391</v>
@@ -3585,7 +3585,7 @@
         <v>11</v>
       </c>
       <c r="R38">
-        <v>-1.2355179786682129</v>
+        <v>-0.89263790845870972</v>
       </c>
       <c r="S38" t="b">
         <v>1</v>
@@ -3644,13 +3644,13 @@
         <v>47</v>
       </c>
       <c r="G39">
-        <v>2.354658842086792</v>
+        <v>1.8565676212310791</v>
       </c>
       <c r="H39">
-        <v>2.1266369819641113</v>
+        <v>1.6767802238464355</v>
       </c>
       <c r="I39">
-        <v>2.6071295738220215</v>
+        <v>2.0556321144104004</v>
       </c>
       <c r="J39">
         <v>26.983379364013672</v>
@@ -3677,7 +3677,7 @@
         <v>11</v>
       </c>
       <c r="R39">
-        <v>-1.2355179786682129</v>
+        <v>-0.89263790845870972</v>
       </c>
       <c r="S39" t="b">
         <v>1</v>
@@ -3736,13 +3736,13 @@
         <v>47</v>
       </c>
       <c r="G40">
-        <v>1.6461821794509888</v>
+        <v>1.2979581356048584</v>
       </c>
       <c r="H40">
-        <v>1.5402425527572632</v>
+        <v>1.2144284248352051</v>
       </c>
       <c r="I40">
-        <v>1.7594084739685059</v>
+        <v>1.3872332572937012</v>
       </c>
       <c r="J40">
         <v>27.206377029418945</v>
@@ -3769,7 +3769,7 @@
         <v>11</v>
       </c>
       <c r="R40">
-        <v>-0.71912401914596558</v>
+        <v>-0.37624391913414001</v>
       </c>
       <c r="S40" t="b">
         <v>1</v>
@@ -3828,13 +3828,13 @@
         <v>47</v>
       </c>
       <c r="G41">
-        <v>1.6461821794509888</v>
+        <v>1.2979581356048584</v>
       </c>
       <c r="H41">
-        <v>1.5402425527572632</v>
+        <v>1.2144284248352051</v>
       </c>
       <c r="I41">
-        <v>1.7594084739685059</v>
+        <v>1.3872332572937012</v>
       </c>
       <c r="J41">
         <v>27.320960998535156</v>
@@ -3861,7 +3861,7 @@
         <v>11</v>
       </c>
       <c r="R41">
-        <v>-0.71912401914596558</v>
+        <v>-0.37624391913414001</v>
       </c>
       <c r="S41" t="b">
         <v>1</v>
@@ -3897,7 +3897,7 @@
         <v>48</v>
       </c>
       <c r="AD41" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
@@ -3920,13 +3920,13 @@
         <v>47</v>
       </c>
       <c r="G42">
-        <v>1.6230413913726807</v>
+        <v>1.279712438583374</v>
       </c>
       <c r="H42">
-        <v>1.3602490425109863</v>
+        <v>1.0725096464157104</v>
       </c>
       <c r="I42">
-        <v>1.9366037845611572</v>
+        <v>1.5269457101821899</v>
       </c>
       <c r="J42">
         <v>27.354499816894531</v>
@@ -3953,7 +3953,7 @@
         <v>11</v>
       </c>
       <c r="R42">
-        <v>-0.69869977235794067</v>
+        <v>-0.3558197021484375</v>
       </c>
       <c r="S42" t="b">
         <v>1</v>
@@ -4012,13 +4012,13 @@
         <v>47</v>
       </c>
       <c r="G43">
-        <v>1.6230413913726807</v>
+        <v>1.279712438583374</v>
       </c>
       <c r="H43">
-        <v>1.3602490425109863</v>
+        <v>1.0725096464157104</v>
       </c>
       <c r="I43">
-        <v>1.9366037845611572</v>
+        <v>1.5269457101821899</v>
       </c>
       <c r="J43">
         <v>27.737514495849609</v>
@@ -4045,7 +4045,7 @@
         <v>11</v>
       </c>
       <c r="R43">
-        <v>-0.69869977235794067</v>
+        <v>-0.3558197021484375</v>
       </c>
       <c r="S43" t="b">
         <v>1</v>
@@ -4104,13 +4104,13 @@
         <v>47</v>
       </c>
       <c r="G44">
-        <v>1.6230413913726807</v>
+        <v>1.279712438583374</v>
       </c>
       <c r="H44">
-        <v>1.3602490425109863</v>
+        <v>1.0725096464157104</v>
       </c>
       <c r="I44">
-        <v>1.9366037845611572</v>
+        <v>1.5269457101821899</v>
       </c>
       <c r="J44">
         <v>27.837169647216797</v>
@@ -4137,7 +4137,7 @@
         <v>11</v>
       </c>
       <c r="R44">
-        <v>-0.69869977235794067</v>
+        <v>-0.3558197021484375</v>
       </c>
       <c r="S44" t="b">
         <v>1</v>
@@ -4173,7 +4173,7 @@
         <v>48</v>
       </c>
       <c r="AD44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
@@ -4357,7 +4357,7 @@
         <v>48</v>
       </c>
       <c r="AD46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
@@ -5116,13 +5116,13 @@
         <v>47</v>
       </c>
       <c r="G55">
-        <v>1.2682859897613525</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>0.84562665224075317</v>
+        <v>0.66674762964248657</v>
       </c>
       <c r="I55">
-        <v>1.9021979570388794</v>
+        <v>1.4998178482055664</v>
       </c>
       <c r="J55">
         <v>27.850744247436523</v>
@@ -5149,7 +5149,7 @@
         <v>11</v>
       </c>
       <c r="R55">
-        <v>-0.34288010001182556</v>
+        <v>0</v>
       </c>
       <c r="S55" t="b">
         <v>1</v>
@@ -5208,13 +5208,13 @@
         <v>47</v>
       </c>
       <c r="G56">
-        <v>1.2682859897613525</v>
+        <v>1</v>
       </c>
       <c r="H56">
-        <v>0.84562665224075317</v>
+        <v>0.66674762964248657</v>
       </c>
       <c r="I56">
-        <v>1.9021979570388794</v>
+        <v>1.4998178482055664</v>
       </c>
       <c r="J56">
         <v>27.190851211547852</v>
@@ -5241,7 +5241,7 @@
         <v>11</v>
       </c>
       <c r="R56">
-        <v>-0.34288010001182556</v>
+        <v>0</v>
       </c>
       <c r="S56" t="b">
         <v>1</v>
@@ -5276,16 +5276,19 @@
       <c r="AC56" t="s">
         <v>48</v>
       </c>
+      <c r="AD56" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D57" t="s">
         <v>45</v>
@@ -5296,32 +5299,32 @@
       <c r="F57" t="s">
         <v>47</v>
       </c>
-      <c r="G57">
-        <v>6.3744287490844727</v>
-      </c>
-      <c r="H57">
-        <v>4.6767382621765137</v>
-      </c>
-      <c r="I57">
-        <v>8.6883935928344727</v>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" t="s">
+        <v>11</v>
       </c>
       <c r="J57">
-        <v>24.779863357543945</v>
+        <v>14.948566436767578</v>
       </c>
       <c r="K57">
-        <v>24.727378845214844</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L57">
-        <v>7.4224308133125305E-2</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M57" t="s">
         <v>11</v>
       </c>
-      <c r="N57">
-        <v>10.614443778991699</v>
-      </c>
-      <c r="O57">
-        <v>0.44679340720176697</v>
+      <c r="N57" t="s">
+        <v>11</v>
+      </c>
+      <c r="O57" t="s">
+        <v>11</v>
       </c>
       <c r="P57" t="s">
         <v>11</v>
@@ -5329,14 +5332,14 @@
       <c r="Q57" t="s">
         <v>11</v>
       </c>
-      <c r="R57">
-        <v>-2.6722960472106934</v>
+      <c r="R57" t="s">
+        <v>11</v>
       </c>
       <c r="S57" t="b">
         <v>1</v>
       </c>
       <c r="T57">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U57" t="b">
         <v>1</v>
@@ -5345,13 +5348,13 @@
         <v>3</v>
       </c>
       <c r="W57">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="X57">
         <v>1</v>
       </c>
       <c r="Y57">
-        <v>89.760971069335938</v>
+        <v>85.889266967773438</v>
       </c>
       <c r="Z57" t="s">
         <v>11</v>
@@ -5363,18 +5366,21 @@
         <v>11</v>
       </c>
       <c r="AC57" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD57" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
         <v>45</v>
@@ -5385,32 +5391,32 @@
       <c r="F58" t="s">
         <v>47</v>
       </c>
-      <c r="G58">
-        <v>6.3744287490844727</v>
-      </c>
-      <c r="H58">
-        <v>4.6767382621765137</v>
-      </c>
-      <c r="I58">
-        <v>8.6883935928344727</v>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" t="s">
+        <v>11</v>
       </c>
       <c r="J58">
-        <v>24.674894332885742</v>
+        <v>14.247366905212402</v>
       </c>
       <c r="K58">
-        <v>24.727378845214844</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L58">
-        <v>7.4224308133125305E-2</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M58" t="s">
         <v>11</v>
       </c>
-      <c r="N58">
-        <v>10.614443778991699</v>
-      </c>
-      <c r="O58">
-        <v>0.44679340720176697</v>
+      <c r="N58" t="s">
+        <v>11</v>
+      </c>
+      <c r="O58" t="s">
+        <v>11</v>
       </c>
       <c r="P58" t="s">
         <v>11</v>
@@ -5418,14 +5424,14 @@
       <c r="Q58" t="s">
         <v>11</v>
       </c>
-      <c r="R58">
-        <v>-2.6722960472106934</v>
+      <c r="R58" t="s">
+        <v>11</v>
       </c>
       <c r="S58" t="b">
         <v>1</v>
       </c>
       <c r="T58">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U58" t="b">
         <v>1</v>
@@ -5434,13 +5440,13 @@
         <v>3</v>
       </c>
       <c r="W58">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X58">
         <v>1</v>
       </c>
       <c r="Y58">
-        <v>89.91845703125</v>
+        <v>85.143783569335938</v>
       </c>
       <c r="Z58" t="s">
         <v>11</v>
@@ -5452,18 +5458,21 @@
         <v>11</v>
       </c>
       <c r="AC58" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD58" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B59" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D59" t="s">
         <v>45</v>
@@ -5474,32 +5483,32 @@
       <c r="F59" t="s">
         <v>47</v>
       </c>
-      <c r="G59">
-        <v>5.1909804344177246</v>
-      </c>
-      <c r="H59">
-        <v>3.0574984550476074</v>
-      </c>
-      <c r="I59">
-        <v>8.8131780624389648</v>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" t="s">
+        <v>11</v>
       </c>
       <c r="J59">
-        <v>25.692060470581055</v>
+        <v>14.534880638122559</v>
       </c>
       <c r="K59">
-        <v>26.205427169799805</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L59">
-        <v>0.72601014375686646</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M59" t="s">
         <v>11</v>
       </c>
-      <c r="N59">
-        <v>10.910732269287109</v>
-      </c>
-      <c r="O59">
-        <v>0.76365530490875244</v>
+      <c r="N59" t="s">
+        <v>11</v>
+      </c>
+      <c r="O59" t="s">
+        <v>11</v>
       </c>
       <c r="P59" t="s">
         <v>11</v>
@@ -5507,14 +5516,14 @@
       <c r="Q59" t="s">
         <v>11</v>
       </c>
-      <c r="R59">
-        <v>-2.376007080078125</v>
+      <c r="R59" t="s">
+        <v>11</v>
       </c>
       <c r="S59" t="b">
         <v>1</v>
       </c>
       <c r="T59">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U59" t="b">
         <v>1</v>
@@ -5523,13 +5532,13 @@
         <v>3</v>
       </c>
       <c r="W59">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="X59">
         <v>1</v>
       </c>
       <c r="Y59">
-        <v>89.169342041015625</v>
+        <v>85.883453369140625</v>
       </c>
       <c r="Z59" t="s">
         <v>11</v>
@@ -5541,15 +5550,18 @@
         <v>11</v>
       </c>
       <c r="AC59" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
         <v>44</v>
@@ -5564,31 +5576,31 @@
         <v>47</v>
       </c>
       <c r="G60">
-        <v>5.1909804344177246</v>
+        <v>2.6037623882293701</v>
       </c>
       <c r="H60">
-        <v>3.0574984550476074</v>
+        <v>1.9103068113327026</v>
       </c>
       <c r="I60">
-        <v>8.8131780624389648</v>
+        <v>3.5489473342895508</v>
       </c>
       <c r="J60">
-        <v>26.718793869018555</v>
+        <v>24.779863357543945</v>
       </c>
       <c r="K60">
-        <v>26.205427169799805</v>
+        <v>24.727378845214844</v>
       </c>
       <c r="L60">
-        <v>0.72601014375686646</v>
+        <v>7.4224308133125305E-2</v>
       </c>
       <c r="M60" t="s">
         <v>11</v>
       </c>
       <c r="N60">
-        <v>10.910732269287109</v>
+        <v>10.614443778991699</v>
       </c>
       <c r="O60">
-        <v>0.76365530490875244</v>
+        <v>0.44679340720176697</v>
       </c>
       <c r="P60" t="s">
         <v>11</v>
@@ -5597,7 +5609,7 @@
         <v>11</v>
       </c>
       <c r="R60">
-        <v>-2.376007080078125</v>
+        <v>-1.380597710609436</v>
       </c>
       <c r="S60" t="b">
         <v>1</v>
@@ -5612,13 +5624,13 @@
         <v>3</v>
       </c>
       <c r="W60">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="X60">
         <v>1</v>
       </c>
       <c r="Y60">
-        <v>89.615737915039062</v>
+        <v>89.760971069335938</v>
       </c>
       <c r="Z60" t="s">
         <v>11</v>
@@ -5630,15 +5642,18 @@
         <v>11</v>
       </c>
       <c r="AC60" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
         <v>44</v>
@@ -5653,31 +5668,31 @@
         <v>47</v>
       </c>
       <c r="G61">
-        <v>3.6847128868103027</v>
+        <v>2.6037623882293701</v>
       </c>
       <c r="H61">
-        <v>2.9759521484375</v>
+        <v>1.9103068113327026</v>
       </c>
       <c r="I61">
-        <v>4.5622739791870117</v>
+        <v>3.5489473342895508</v>
       </c>
       <c r="J61">
-        <v>26.025688171386719</v>
+        <v>24.674894332885742</v>
       </c>
       <c r="K61">
-        <v>25.985088348388672</v>
+        <v>24.727378845214844</v>
       </c>
       <c r="L61">
-        <v>5.7416819036006927E-2</v>
+        <v>7.4224308133125305E-2</v>
       </c>
       <c r="M61" t="s">
         <v>11</v>
       </c>
       <c r="N61">
-        <v>11.405187606811523</v>
+        <v>10.614443778991699</v>
       </c>
       <c r="O61">
-        <v>0.30820083618164062</v>
+        <v>0.44679340720176697</v>
       </c>
       <c r="P61" t="s">
         <v>11</v>
@@ -5686,7 +5701,7 @@
         <v>11</v>
       </c>
       <c r="R61">
-        <v>-1.8815522193908691</v>
+        <v>-1.380597710609436</v>
       </c>
       <c r="S61" t="b">
         <v>1</v>
@@ -5701,13 +5716,13 @@
         <v>3</v>
       </c>
       <c r="W61">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X61">
         <v>1</v>
       </c>
       <c r="Y61">
-        <v>90.063064575195312</v>
+        <v>89.91845703125</v>
       </c>
       <c r="Z61" t="s">
         <v>11</v>
@@ -5719,15 +5734,18 @@
         <v>11</v>
       </c>
       <c r="AC61" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD61" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
         <v>44</v>
@@ -5742,31 +5760,31 @@
         <v>47</v>
       </c>
       <c r="G62">
-        <v>3.6847128868103027</v>
+        <v>2.1203594207763672</v>
       </c>
       <c r="H62">
-        <v>2.9759521484375</v>
+        <v>1.2488961219787598</v>
       </c>
       <c r="I62">
-        <v>4.5622739791870117</v>
+        <v>3.5999181270599365</v>
       </c>
       <c r="J62">
-        <v>25.944488525390625</v>
+        <v>25.692060470581055</v>
       </c>
       <c r="K62">
-        <v>25.985088348388672</v>
+        <v>26.205427169799805</v>
       </c>
       <c r="L62">
-        <v>5.7416819036006927E-2</v>
+        <v>0.72601014375686646</v>
       </c>
       <c r="M62" t="s">
         <v>11</v>
       </c>
       <c r="N62">
-        <v>11.405187606811523</v>
+        <v>10.910732269287109</v>
       </c>
       <c r="O62">
-        <v>0.30820083618164062</v>
+        <v>0.76365530490875244</v>
       </c>
       <c r="P62" t="s">
         <v>11</v>
@@ -5775,7 +5793,7 @@
         <v>11</v>
       </c>
       <c r="R62">
-        <v>-1.8815522193908691</v>
+        <v>-1.0843087434768677</v>
       </c>
       <c r="S62" t="b">
         <v>1</v>
@@ -5796,7 +5814,7 @@
         <v>1</v>
       </c>
       <c r="Y62">
-        <v>89.765937805175781</v>
+        <v>89.169342041015625</v>
       </c>
       <c r="Z62" t="s">
         <v>11</v>
@@ -5808,18 +5826,21 @@
         <v>11</v>
       </c>
       <c r="AC62" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD62" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C63" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D63" t="s">
         <v>45</v>
@@ -5830,32 +5851,32 @@
       <c r="F63" t="s">
         <v>47</v>
       </c>
-      <c r="G63" t="s">
-        <v>11</v>
-      </c>
-      <c r="H63" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" t="s">
-        <v>11</v>
+      <c r="G63">
+        <v>2.1203594207763672</v>
+      </c>
+      <c r="H63">
+        <v>1.2488961219787598</v>
+      </c>
+      <c r="I63">
+        <v>3.5999181270599365</v>
       </c>
       <c r="J63">
-        <v>14.948566436767578</v>
+        <v>26.718793869018555</v>
       </c>
       <c r="K63">
-        <v>14.576937675476074</v>
+        <v>26.205427169799805</v>
       </c>
       <c r="L63">
-        <v>0.35248661041259766</v>
+        <v>0.72601014375686646</v>
       </c>
       <c r="M63" t="s">
         <v>11</v>
       </c>
-      <c r="N63" t="s">
-        <v>11</v>
-      </c>
-      <c r="O63" t="s">
-        <v>11</v>
+      <c r="N63">
+        <v>10.910732269287109</v>
+      </c>
+      <c r="O63">
+        <v>0.76365530490875244</v>
       </c>
       <c r="P63" t="s">
         <v>11</v>
@@ -5863,14 +5884,14 @@
       <c r="Q63" t="s">
         <v>11</v>
       </c>
-      <c r="R63" t="s">
-        <v>11</v>
+      <c r="R63">
+        <v>-1.0843087434768677</v>
       </c>
       <c r="S63" t="b">
         <v>1</v>
       </c>
       <c r="T63">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U63" t="b">
         <v>1</v>
@@ -5879,13 +5900,13 @@
         <v>3</v>
       </c>
       <c r="W63">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="X63">
         <v>1</v>
       </c>
       <c r="Y63">
-        <v>85.889266967773438</v>
+        <v>89.615737915039062</v>
       </c>
       <c r="Z63" t="s">
         <v>11</v>
@@ -5897,18 +5918,21 @@
         <v>11</v>
       </c>
       <c r="AC63" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD63" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D64" t="s">
         <v>45</v>
@@ -5919,32 +5943,32 @@
       <c r="F64" t="s">
         <v>47</v>
       </c>
-      <c r="G64" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" t="s">
-        <v>11</v>
+      <c r="G64">
+        <v>1.5050942897796631</v>
+      </c>
+      <c r="H64">
+        <v>1.2155869007110596</v>
+      </c>
+      <c r="I64">
+        <v>1.8635516166687012</v>
       </c>
       <c r="J64">
-        <v>14.247366905212402</v>
+        <v>26.025688171386719</v>
       </c>
       <c r="K64">
-        <v>14.576937675476074</v>
+        <v>25.985088348388672</v>
       </c>
       <c r="L64">
-        <v>0.35248661041259766</v>
+        <v>5.7416819036006927E-2</v>
       </c>
       <c r="M64" t="s">
         <v>11</v>
       </c>
-      <c r="N64" t="s">
-        <v>11</v>
-      </c>
-      <c r="O64" t="s">
-        <v>11</v>
+      <c r="N64">
+        <v>11.405187606811523</v>
+      </c>
+      <c r="O64">
+        <v>0.30820083618164062</v>
       </c>
       <c r="P64" t="s">
         <v>11</v>
@@ -5952,14 +5976,14 @@
       <c r="Q64" t="s">
         <v>11</v>
       </c>
-      <c r="R64" t="s">
-        <v>11</v>
+      <c r="R64">
+        <v>-0.58985394239425659</v>
       </c>
       <c r="S64" t="b">
         <v>1</v>
       </c>
       <c r="T64">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U64" t="b">
         <v>1</v>
@@ -5968,13 +5992,13 @@
         <v>3</v>
       </c>
       <c r="W64">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="X64">
         <v>1</v>
       </c>
       <c r="Y64">
-        <v>85.143783569335938</v>
+        <v>90.063064575195312</v>
       </c>
       <c r="Z64" t="s">
         <v>11</v>
@@ -5988,16 +6012,19 @@
       <c r="AC64" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C65" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D65" t="s">
         <v>45</v>
@@ -6008,32 +6035,32 @@
       <c r="F65" t="s">
         <v>47</v>
       </c>
-      <c r="G65" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" t="s">
-        <v>11</v>
+      <c r="G65">
+        <v>1.5050942897796631</v>
+      </c>
+      <c r="H65">
+        <v>1.2155869007110596</v>
+      </c>
+      <c r="I65">
+        <v>1.8635516166687012</v>
       </c>
       <c r="J65">
-        <v>14.534880638122559</v>
+        <v>25.944488525390625</v>
       </c>
       <c r="K65">
-        <v>14.576937675476074</v>
+        <v>25.985088348388672</v>
       </c>
       <c r="L65">
-        <v>0.35248661041259766</v>
+        <v>5.7416819036006927E-2</v>
       </c>
       <c r="M65" t="s">
         <v>11</v>
       </c>
-      <c r="N65" t="s">
-        <v>11</v>
-      </c>
-      <c r="O65" t="s">
-        <v>11</v>
+      <c r="N65">
+        <v>11.405187606811523</v>
+      </c>
+      <c r="O65">
+        <v>0.30820083618164062</v>
       </c>
       <c r="P65" t="s">
         <v>11</v>
@@ -6041,14 +6068,14 @@
       <c r="Q65" t="s">
         <v>11</v>
       </c>
-      <c r="R65" t="s">
-        <v>11</v>
+      <c r="R65">
+        <v>-0.58985394239425659</v>
       </c>
       <c r="S65" t="b">
         <v>1</v>
       </c>
       <c r="T65">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U65" t="b">
         <v>1</v>
@@ -6057,13 +6084,13 @@
         <v>3</v>
       </c>
       <c r="W65">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="X65">
         <v>1</v>
       </c>
       <c r="Y65">
-        <v>85.883453369140625</v>
+        <v>89.765937805175781</v>
       </c>
       <c r="Z65" t="s">
         <v>11</v>
@@ -6077,13 +6104,16 @@
       <c r="AC65" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
         <v>62</v>
@@ -6107,13 +6137,13 @@
         <v>11</v>
       </c>
       <c r="J66">
-        <v>13.801394462585449</v>
+        <v>14.948566436767578</v>
       </c>
       <c r="K66">
-        <v>14.112935066223145</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L66">
-        <v>0.44058495759963989</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M66" t="s">
         <v>11</v>
@@ -6152,7 +6182,7 @@
         <v>1</v>
       </c>
       <c r="Y66">
-        <v>85.286911010742188</v>
+        <v>85.889266967773438</v>
       </c>
       <c r="Z66" t="s">
         <v>11</v>
@@ -6166,13 +6196,16 @@
       <c r="AC66" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD66" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C67" t="s">
         <v>62</v>
@@ -6196,13 +6229,13 @@
         <v>11</v>
       </c>
       <c r="J67">
-        <v>14.42447566986084</v>
+        <v>14.247366905212402</v>
       </c>
       <c r="K67">
-        <v>14.112935066223145</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L67">
-        <v>0.44058495759963989</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M67" t="s">
         <v>11</v>
@@ -6235,13 +6268,13 @@
         <v>3</v>
       </c>
       <c r="W67">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X67">
         <v>1</v>
       </c>
       <c r="Y67">
-        <v>86.042121887207031</v>
+        <v>85.143783569335938</v>
       </c>
       <c r="Z67" t="s">
         <v>11</v>
@@ -6255,13 +6288,16 @@
       <c r="AC67" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
         <v>62</v>
@@ -6285,13 +6321,13 @@
         <v>11</v>
       </c>
       <c r="J68">
-        <v>15.462143898010254</v>
+        <v>14.534880638122559</v>
       </c>
       <c r="K68">
-        <v>15.294694900512695</v>
+        <v>14.576937675476074</v>
       </c>
       <c r="L68">
-        <v>0.23680931329727173</v>
+        <v>0.35248661041259766</v>
       </c>
       <c r="M68" t="s">
         <v>11</v>
@@ -6324,13 +6360,13 @@
         <v>3</v>
       </c>
       <c r="W68">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="X68">
         <v>1</v>
       </c>
       <c r="Y68">
-        <v>85.739601135253906</v>
+        <v>85.883453369140625</v>
       </c>
       <c r="Z68" t="s">
         <v>11</v>
@@ -6344,13 +6380,16 @@
       <c r="AC68" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
         <v>62</v>
@@ -6374,13 +6413,13 @@
         <v>11</v>
       </c>
       <c r="J69">
-        <v>15.12724494934082</v>
+        <v>13.801394462585449</v>
       </c>
       <c r="K69">
-        <v>15.294694900512695</v>
+        <v>14.112935066223145</v>
       </c>
       <c r="L69">
-        <v>0.23680931329727173</v>
+        <v>0.44058495759963989</v>
       </c>
       <c r="M69" t="s">
         <v>11</v>
@@ -6419,7 +6458,7 @@
         <v>1</v>
       </c>
       <c r="Y69">
-        <v>85.739601135253906</v>
+        <v>85.286911010742188</v>
       </c>
       <c r="Z69" t="s">
         <v>11</v>
@@ -6433,13 +6472,16 @@
       <c r="AC69" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD69" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>62</v>
@@ -6463,13 +6505,13 @@
         <v>11</v>
       </c>
       <c r="J70">
-        <v>14.280258178710938</v>
+        <v>14.42447566986084</v>
       </c>
       <c r="K70">
-        <v>14.579899787902832</v>
+        <v>14.112935066223145</v>
       </c>
       <c r="L70">
-        <v>0.3028053343296051</v>
+        <v>0.44058495759963989</v>
       </c>
       <c r="M70" t="s">
         <v>11</v>
@@ -6502,13 +6544,13 @@
         <v>3</v>
       </c>
       <c r="W70">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X70">
         <v>1</v>
       </c>
       <c r="Y70">
-        <v>85.738868713378906</v>
+        <v>86.042121887207031</v>
       </c>
       <c r="Z70" t="s">
         <v>11</v>
@@ -6522,13 +6564,16 @@
       <c r="AC70" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
         <v>62</v>
@@ -6552,13 +6597,13 @@
         <v>11</v>
       </c>
       <c r="J71">
-        <v>14.573671340942383</v>
+        <v>15.462143898010254</v>
       </c>
       <c r="K71">
-        <v>14.579899787902832</v>
+        <v>15.294694900512695</v>
       </c>
       <c r="L71">
-        <v>0.3028053343296051</v>
+        <v>0.23680931329727173</v>
       </c>
       <c r="M71" t="s">
         <v>11</v>
@@ -6591,13 +6636,13 @@
         <v>3</v>
       </c>
       <c r="W71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X71">
         <v>1</v>
       </c>
       <c r="Y71">
-        <v>85.591812133789062</v>
+        <v>85.739601135253906</v>
       </c>
       <c r="Z71" t="s">
         <v>11</v>
@@ -6611,13 +6656,16 @@
       <c r="AC71" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD71" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
         <v>62</v>
@@ -6641,13 +6689,13 @@
         <v>11</v>
       </c>
       <c r="J72">
-        <v>14.885772705078125</v>
+        <v>15.12724494934082</v>
       </c>
       <c r="K72">
-        <v>14.579899787902832</v>
+        <v>15.294694900512695</v>
       </c>
       <c r="L72">
-        <v>0.3028053343296051</v>
+        <v>0.23680931329727173</v>
       </c>
       <c r="M72" t="s">
         <v>11</v>
@@ -6680,13 +6728,13 @@
         <v>3</v>
       </c>
       <c r="W72">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X72">
         <v>1</v>
       </c>
       <c r="Y72">
-        <v>85.591812133789062</v>
+        <v>85.739601135253906</v>
       </c>
       <c r="Z72" t="s">
         <v>11</v>
@@ -6700,16 +6748,19 @@
       <c r="AC72" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C73" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D73" t="s">
         <v>45</v>
@@ -6720,32 +6771,32 @@
       <c r="F73" t="s">
         <v>47</v>
       </c>
-      <c r="G73">
-        <v>0.59230715036392212</v>
-      </c>
-      <c r="H73">
-        <v>0.52589905261993408</v>
-      </c>
-      <c r="I73">
-        <v>0.66710090637207031</v>
+      <c r="G73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" t="s">
+        <v>11</v>
+      </c>
+      <c r="I73" t="s">
+        <v>11</v>
       </c>
       <c r="J73">
-        <v>29.559513092041016</v>
+        <v>14.280258178710938</v>
       </c>
       <c r="K73">
-        <v>29.527490615844727</v>
+        <v>14.579899787902832</v>
       </c>
       <c r="L73">
-        <v>4.3911471962928772E-2</v>
+        <v>0.3028053343296051</v>
       </c>
       <c r="M73" t="s">
         <v>11</v>
       </c>
-      <c r="N73">
-        <v>14.042322158813477</v>
-      </c>
-      <c r="O73">
-        <v>0.17155957221984863</v>
+      <c r="N73" t="s">
+        <v>11</v>
+      </c>
+      <c r="O73" t="s">
+        <v>11</v>
       </c>
       <c r="P73" t="s">
         <v>11</v>
@@ -6753,14 +6804,14 @@
       <c r="Q73" t="s">
         <v>11</v>
       </c>
-      <c r="R73">
-        <v>0.75558263063430786</v>
+      <c r="R73" t="s">
+        <v>11</v>
       </c>
       <c r="S73" t="b">
         <v>1</v>
       </c>
       <c r="T73">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U73" t="b">
         <v>1</v>
@@ -6769,13 +6820,13 @@
         <v>3</v>
       </c>
       <c r="W73">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="X73">
         <v>1</v>
       </c>
       <c r="Y73">
-        <v>89.616653442382812</v>
+        <v>85.738868713378906</v>
       </c>
       <c r="Z73" t="s">
         <v>11</v>
@@ -6789,16 +6840,19 @@
       <c r="AC73" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D74" t="s">
         <v>45</v>
@@ -6809,32 +6863,32 @@
       <c r="F74" t="s">
         <v>47</v>
       </c>
-      <c r="G74">
-        <v>0.59230715036392212</v>
-      </c>
-      <c r="H74">
-        <v>0.52589905261993408</v>
-      </c>
-      <c r="I74">
-        <v>0.66710090637207031</v>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" t="s">
+        <v>11</v>
+      </c>
+      <c r="I74" t="s">
+        <v>11</v>
       </c>
       <c r="J74">
-        <v>29.545522689819336</v>
+        <v>14.573671340942383</v>
       </c>
       <c r="K74">
-        <v>29.527490615844727</v>
+        <v>14.579899787902832</v>
       </c>
       <c r="L74">
-        <v>4.3911471962928772E-2</v>
+        <v>0.3028053343296051</v>
       </c>
       <c r="M74" t="s">
         <v>11</v>
       </c>
-      <c r="N74">
-        <v>14.042322158813477</v>
-      </c>
-      <c r="O74">
-        <v>0.17155957221984863</v>
+      <c r="N74" t="s">
+        <v>11</v>
+      </c>
+      <c r="O74" t="s">
+        <v>11</v>
       </c>
       <c r="P74" t="s">
         <v>11</v>
@@ -6842,14 +6896,14 @@
       <c r="Q74" t="s">
         <v>11</v>
       </c>
-      <c r="R74">
-        <v>0.75558263063430786</v>
+      <c r="R74" t="s">
+        <v>11</v>
       </c>
       <c r="S74" t="b">
         <v>1</v>
       </c>
       <c r="T74">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U74" t="b">
         <v>1</v>
@@ -6858,13 +6912,13 @@
         <v>3</v>
       </c>
       <c r="W74">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="X74">
         <v>1</v>
       </c>
       <c r="Y74">
-        <v>89.616653442382812</v>
+        <v>85.591812133789062</v>
       </c>
       <c r="Z74" t="s">
         <v>11</v>
@@ -6878,16 +6932,19 @@
       <c r="AC74" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD74" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D75" t="s">
         <v>45</v>
@@ -6898,32 +6955,32 @@
       <c r="F75" t="s">
         <v>47</v>
       </c>
-      <c r="G75">
-        <v>0.59230715036392212</v>
-      </c>
-      <c r="H75">
-        <v>0.52589905261993408</v>
-      </c>
-      <c r="I75">
-        <v>0.66710090637207031</v>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" t="s">
+        <v>11</v>
+      </c>
+      <c r="I75" t="s">
+        <v>11</v>
       </c>
       <c r="J75">
-        <v>29.477432250976562</v>
+        <v>14.885772705078125</v>
       </c>
       <c r="K75">
-        <v>29.527490615844727</v>
+        <v>14.579899787902832</v>
       </c>
       <c r="L75">
-        <v>4.3911471962928772E-2</v>
+        <v>0.3028053343296051</v>
       </c>
       <c r="M75" t="s">
         <v>11</v>
       </c>
-      <c r="N75">
-        <v>14.042322158813477</v>
-      </c>
-      <c r="O75">
-        <v>0.17155957221984863</v>
+      <c r="N75" t="s">
+        <v>11</v>
+      </c>
+      <c r="O75" t="s">
+        <v>11</v>
       </c>
       <c r="P75" t="s">
         <v>11</v>
@@ -6931,14 +6988,14 @@
       <c r="Q75" t="s">
         <v>11</v>
       </c>
-      <c r="R75">
-        <v>0.75558263063430786</v>
+      <c r="R75" t="s">
+        <v>11</v>
       </c>
       <c r="S75" t="b">
         <v>1</v>
       </c>
       <c r="T75">
-        <v>10962.467447916668</v>
+        <v>9869.0254278273824</v>
       </c>
       <c r="U75" t="b">
         <v>1</v>
@@ -6947,16 +7004,16 @@
         <v>3</v>
       </c>
       <c r="W75">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="X75">
         <v>1</v>
       </c>
       <c r="Y75">
-        <v>89.611831665039062</v>
-      </c>
-      <c r="Z75">
-        <v>84.242965698242188</v>
+        <v>85.591812133789062</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>11</v>
       </c>
       <c r="AA75" t="s">
         <v>11</v>
@@ -6967,13 +7024,16 @@
       <c r="AC75" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C76" t="s">
         <v>44</v>
@@ -6988,31 +7048,31 @@
         <v>47</v>
       </c>
       <c r="G76">
-        <v>2.4481606483459473</v>
+        <v>0.24193963408470154</v>
       </c>
       <c r="H76">
-        <v>2.0776131153106689</v>
+        <v>0.21481393277645111</v>
       </c>
       <c r="I76">
-        <v>2.8847966194152832</v>
+        <v>0.27249065041542053</v>
       </c>
       <c r="J76">
-        <v>26.545694351196289</v>
+        <v>29.559513092041016</v>
       </c>
       <c r="K76">
-        <v>26.57196044921875</v>
+        <v>29.527490615844727</v>
       </c>
       <c r="L76">
-        <v>0.20349620282649994</v>
+        <v>4.3911471962928772E-2</v>
       </c>
       <c r="M76" t="s">
         <v>11</v>
       </c>
       <c r="N76">
-        <v>11.995041847229004</v>
+        <v>14.042322158813477</v>
       </c>
       <c r="O76">
-        <v>0.23677127063274384</v>
+        <v>0.17155957221984863</v>
       </c>
       <c r="P76" t="s">
         <v>11</v>
@@ -7021,7 +7081,7 @@
         <v>11</v>
       </c>
       <c r="R76">
-        <v>-1.2916983366012573</v>
+        <v>2.04728102684021</v>
       </c>
       <c r="S76" t="b">
         <v>1</v>
@@ -7036,13 +7096,13 @@
         <v>3</v>
       </c>
       <c r="W76">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="X76">
         <v>1</v>
       </c>
       <c r="Y76">
-        <v>90.2083740234375</v>
+        <v>89.616653442382812</v>
       </c>
       <c r="Z76" t="s">
         <v>11</v>
@@ -7056,13 +7116,16 @@
       <c r="AC76" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD76" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C77" t="s">
         <v>44</v>
@@ -7077,31 +7140,31 @@
         <v>47</v>
       </c>
       <c r="G77">
-        <v>2.4481606483459473</v>
+        <v>0.24193963408470154</v>
       </c>
       <c r="H77">
-        <v>2.0776131153106689</v>
+        <v>0.21481393277645111</v>
       </c>
       <c r="I77">
-        <v>2.8847966194152832</v>
+        <v>0.27249065041542053</v>
       </c>
       <c r="J77">
-        <v>26.382871627807617</v>
+        <v>29.545522689819336</v>
       </c>
       <c r="K77">
-        <v>26.57196044921875</v>
+        <v>29.527490615844727</v>
       </c>
       <c r="L77">
-        <v>0.20349620282649994</v>
+        <v>4.3911471962928772E-2</v>
       </c>
       <c r="M77" t="s">
         <v>11</v>
       </c>
       <c r="N77">
-        <v>11.995041847229004</v>
+        <v>14.042322158813477</v>
       </c>
       <c r="O77">
-        <v>0.23677127063274384</v>
+        <v>0.17155957221984863</v>
       </c>
       <c r="P77" t="s">
         <v>11</v>
@@ -7110,7 +7173,7 @@
         <v>11</v>
       </c>
       <c r="R77">
-        <v>-1.2916983366012573</v>
+        <v>2.04728102684021</v>
       </c>
       <c r="S77" t="b">
         <v>1</v>
@@ -7125,13 +7188,13 @@
         <v>3</v>
       </c>
       <c r="W77">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="X77">
         <v>1</v>
       </c>
       <c r="Y77">
-        <v>90.36572265625</v>
+        <v>89.616653442382812</v>
       </c>
       <c r="Z77" t="s">
         <v>11</v>
@@ -7145,13 +7208,16 @@
       <c r="AC77" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD77" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C78" t="s">
         <v>44</v>
@@ -7166,31 +7232,31 @@
         <v>47</v>
       </c>
       <c r="G78">
-        <v>2.4481606483459473</v>
+        <v>0.24193963408470154</v>
       </c>
       <c r="H78">
-        <v>2.0776131153106689</v>
+        <v>0.21481393277645111</v>
       </c>
       <c r="I78">
-        <v>2.8847966194152832</v>
+        <v>0.27249065041542053</v>
       </c>
       <c r="J78">
-        <v>26.787313461303711</v>
+        <v>29.477432250976562</v>
       </c>
       <c r="K78">
-        <v>26.57196044921875</v>
+        <v>29.527490615844727</v>
       </c>
       <c r="L78">
-        <v>0.20349620282649994</v>
+        <v>4.3911471962928772E-2</v>
       </c>
       <c r="M78" t="s">
         <v>11</v>
       </c>
       <c r="N78">
-        <v>11.995041847229004</v>
+        <v>14.042322158813477</v>
       </c>
       <c r="O78">
-        <v>0.23677127063274384</v>
+        <v>0.17155957221984863</v>
       </c>
       <c r="P78" t="s">
         <v>11</v>
@@ -7199,7 +7265,7 @@
         <v>11</v>
       </c>
       <c r="R78">
-        <v>-1.2916983366012573</v>
+        <v>2.04728102684021</v>
       </c>
       <c r="S78" t="b">
         <v>1</v>
@@ -7214,16 +7280,16 @@
         <v>3</v>
       </c>
       <c r="W78">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="X78">
         <v>1</v>
       </c>
       <c r="Y78">
-        <v>90.514816284179688</v>
-      </c>
-      <c r="Z78" t="s">
-        <v>11</v>
+        <v>89.611831665039062</v>
+      </c>
+      <c r="Z78">
+        <v>84.242965698242188</v>
       </c>
       <c r="AA78" t="s">
         <v>11</v>
@@ -7234,16 +7300,19 @@
       <c r="AC78" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D79" t="s">
         <v>45</v>
@@ -7254,32 +7323,32 @@
       <c r="F79" t="s">
         <v>47</v>
       </c>
-      <c r="G79" t="s">
-        <v>11</v>
-      </c>
-      <c r="H79" t="s">
-        <v>11</v>
-      </c>
-      <c r="I79" t="s">
-        <v>11</v>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>0.84864246845245361</v>
+      </c>
+      <c r="I79">
+        <v>1.1783525943756104</v>
       </c>
       <c r="J79">
-        <v>15.40233039855957</v>
+        <v>26.545694351196289</v>
       </c>
       <c r="K79">
-        <v>15.485165596008301</v>
+        <v>26.57196044921875</v>
       </c>
       <c r="L79">
-        <v>0.16584472358226776</v>
+        <v>0.20349620282649994</v>
       </c>
       <c r="M79" t="s">
         <v>11</v>
       </c>
-      <c r="N79" t="s">
-        <v>11</v>
-      </c>
-      <c r="O79" t="s">
-        <v>11</v>
+      <c r="N79">
+        <v>11.995041847229004</v>
+      </c>
+      <c r="O79">
+        <v>0.23677127063274384</v>
       </c>
       <c r="P79" t="s">
         <v>11</v>
@@ -7287,14 +7356,14 @@
       <c r="Q79" t="s">
         <v>11</v>
       </c>
-      <c r="R79" t="s">
-        <v>11</v>
+      <c r="R79">
+        <v>0</v>
       </c>
       <c r="S79" t="b">
         <v>1</v>
       </c>
       <c r="T79">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U79" t="b">
         <v>1</v>
@@ -7303,13 +7372,13 @@
         <v>3</v>
       </c>
       <c r="W79">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="X79">
         <v>1</v>
       </c>
       <c r="Y79">
-        <v>84.99468994140625</v>
+        <v>90.2083740234375</v>
       </c>
       <c r="Z79" t="s">
         <v>11</v>
@@ -7323,16 +7392,19 @@
       <c r="AC79" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD79" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D80" t="s">
         <v>45</v>
@@ -7343,32 +7415,32 @@
       <c r="F80" t="s">
         <v>47</v>
       </c>
-      <c r="G80" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" t="s">
-        <v>11</v>
-      </c>
-      <c r="I80" t="s">
-        <v>11</v>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>0.84864246845245361</v>
+      </c>
+      <c r="I80">
+        <v>1.1783525943756104</v>
       </c>
       <c r="J80">
-        <v>15.676111221313477</v>
+        <v>26.382871627807617</v>
       </c>
       <c r="K80">
-        <v>15.485165596008301</v>
+        <v>26.57196044921875</v>
       </c>
       <c r="L80">
-        <v>0.16584472358226776</v>
+        <v>0.20349620282649994</v>
       </c>
       <c r="M80" t="s">
         <v>11</v>
       </c>
-      <c r="N80" t="s">
-        <v>11</v>
-      </c>
-      <c r="O80" t="s">
-        <v>11</v>
+      <c r="N80">
+        <v>11.995041847229004</v>
+      </c>
+      <c r="O80">
+        <v>0.23677127063274384</v>
       </c>
       <c r="P80" t="s">
         <v>11</v>
@@ -7376,14 +7448,14 @@
       <c r="Q80" t="s">
         <v>11</v>
       </c>
-      <c r="R80" t="s">
-        <v>11</v>
+      <c r="R80">
+        <v>0</v>
       </c>
       <c r="S80" t="b">
         <v>1</v>
       </c>
       <c r="T80">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U80" t="b">
         <v>1</v>
@@ -7392,13 +7464,13 @@
         <v>3</v>
       </c>
       <c r="W80">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="X80">
         <v>1</v>
       </c>
       <c r="Y80">
-        <v>85.143783569335938</v>
+        <v>90.36572265625</v>
       </c>
       <c r="Z80" t="s">
         <v>11</v>
@@ -7412,16 +7484,19 @@
       <c r="AC80" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D81" t="s">
         <v>45</v>
@@ -7432,32 +7507,32 @@
       <c r="F81" t="s">
         <v>47</v>
       </c>
-      <c r="G81" t="s">
-        <v>11</v>
-      </c>
-      <c r="H81" t="s">
-        <v>11</v>
-      </c>
-      <c r="I81" t="s">
-        <v>11</v>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>0.84864246845245361</v>
+      </c>
+      <c r="I81">
+        <v>1.1783525943756104</v>
       </c>
       <c r="J81">
-        <v>15.377058982849121</v>
+        <v>26.787313461303711</v>
       </c>
       <c r="K81">
-        <v>15.485165596008301</v>
+        <v>26.57196044921875</v>
       </c>
       <c r="L81">
-        <v>0.16584472358226776</v>
+        <v>0.20349620282649994</v>
       </c>
       <c r="M81" t="s">
         <v>11</v>
       </c>
-      <c r="N81" t="s">
-        <v>11</v>
-      </c>
-      <c r="O81" t="s">
-        <v>11</v>
+      <c r="N81">
+        <v>11.995041847229004</v>
+      </c>
+      <c r="O81">
+        <v>0.23677127063274384</v>
       </c>
       <c r="P81" t="s">
         <v>11</v>
@@ -7465,14 +7540,14 @@
       <c r="Q81" t="s">
         <v>11</v>
       </c>
-      <c r="R81" t="s">
-        <v>11</v>
+      <c r="R81">
+        <v>0</v>
       </c>
       <c r="S81" t="b">
         <v>1</v>
       </c>
       <c r="T81">
-        <v>9869.0254278273824</v>
+        <v>10962.467447916668</v>
       </c>
       <c r="U81" t="b">
         <v>1</v>
@@ -7481,13 +7556,13 @@
         <v>3</v>
       </c>
       <c r="W81">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="X81">
         <v>1</v>
       </c>
       <c r="Y81">
-        <v>85.137771606445312</v>
+        <v>90.514816284179688</v>
       </c>
       <c r="Z81" t="s">
         <v>11</v>
@@ -7501,13 +7576,16 @@
       <c r="AC81" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD81" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C82" t="s">
         <v>62</v>
@@ -7531,13 +7609,13 @@
         <v>11</v>
       </c>
       <c r="J82">
-        <v>14.619338989257812</v>
+        <v>15.40233039855957</v>
       </c>
       <c r="K82">
-        <v>14.576918601989746</v>
+        <v>15.485165596008301</v>
       </c>
       <c r="L82">
-        <v>0.12103687971830368</v>
+        <v>0.16584472358226776</v>
       </c>
       <c r="M82" t="s">
         <v>11</v>
@@ -7570,13 +7648,13 @@
         <v>3</v>
       </c>
       <c r="W82">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X82">
         <v>1</v>
       </c>
       <c r="Y82">
-        <v>86.032585144042969</v>
+        <v>84.99468994140625</v>
       </c>
       <c r="Z82" t="s">
         <v>11</v>
@@ -7590,13 +7668,16 @@
       <c r="AC82" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD82" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C83" t="s">
         <v>62</v>
@@ -7620,13 +7701,13 @@
         <v>11</v>
       </c>
       <c r="J83">
-        <v>14.671034812927246</v>
+        <v>15.676111221313477</v>
       </c>
       <c r="K83">
-        <v>14.576918601989746</v>
+        <v>15.485165596008301</v>
       </c>
       <c r="L83">
-        <v>0.12103687971830368</v>
+        <v>0.16584472358226776</v>
       </c>
       <c r="M83" t="s">
         <v>11</v>
@@ -7659,13 +7740,13 @@
         <v>3</v>
       </c>
       <c r="W83">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X83">
         <v>1</v>
       </c>
       <c r="Y83">
-        <v>86.191207885742188</v>
+        <v>85.143783569335938</v>
       </c>
       <c r="Z83" t="s">
         <v>11</v>
@@ -7679,13 +7760,16 @@
       <c r="AC83" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD83" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C84" t="s">
         <v>62</v>
@@ -7709,13 +7793,13 @@
         <v>11</v>
       </c>
       <c r="J84">
-        <v>14.440381050109863</v>
+        <v>15.377058982849121</v>
       </c>
       <c r="K84">
-        <v>14.576918601989746</v>
+        <v>15.485165596008301</v>
       </c>
       <c r="L84">
-        <v>0.12103687971830368</v>
+        <v>0.16584472358226776</v>
       </c>
       <c r="M84" t="s">
         <v>11</v>
@@ -7748,56 +7832,335 @@
         <v>3</v>
       </c>
       <c r="W84">
+        <v>8</v>
+      </c>
+      <c r="X84">
+        <v>1</v>
+      </c>
+      <c r="Y84">
+        <v>85.137771606445312</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA84" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC84" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD84" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>115</v>
+      </c>
+      <c r="B85" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85" t="s">
+        <v>45</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" t="s">
+        <v>47</v>
+      </c>
+      <c r="G85" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" t="s">
+        <v>11</v>
+      </c>
+      <c r="I85" t="s">
+        <v>11</v>
+      </c>
+      <c r="J85">
+        <v>14.619338989257812</v>
+      </c>
+      <c r="K85">
+        <v>14.576918601989746</v>
+      </c>
+      <c r="L85">
+        <v>0.12103687971830368</v>
+      </c>
+      <c r="M85" t="s">
+        <v>11</v>
+      </c>
+      <c r="N85" t="s">
+        <v>11</v>
+      </c>
+      <c r="O85" t="s">
+        <v>11</v>
+      </c>
+      <c r="P85" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>11</v>
+      </c>
+      <c r="R85" t="s">
+        <v>11</v>
+      </c>
+      <c r="S85" t="b">
+        <v>1</v>
+      </c>
+      <c r="T85">
+        <v>9869.0254278273824</v>
+      </c>
+      <c r="U85" t="b">
+        <v>1</v>
+      </c>
+      <c r="V85">
+        <v>3</v>
+      </c>
+      <c r="W85">
+        <v>9</v>
+      </c>
+      <c r="X85">
+        <v>1</v>
+      </c>
+      <c r="Y85">
+        <v>86.032585144042969</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>116</v>
+      </c>
+      <c r="B86" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" t="s">
+        <v>45</v>
+      </c>
+      <c r="E86" t="s">
+        <v>46</v>
+      </c>
+      <c r="F86" t="s">
+        <v>47</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" t="s">
+        <v>11</v>
+      </c>
+      <c r="I86" t="s">
+        <v>11</v>
+      </c>
+      <c r="J86">
+        <v>14.671034812927246</v>
+      </c>
+      <c r="K86">
+        <v>14.576918601989746</v>
+      </c>
+      <c r="L86">
+        <v>0.12103687971830368</v>
+      </c>
+      <c r="M86" t="s">
+        <v>11</v>
+      </c>
+      <c r="N86" t="s">
+        <v>11</v>
+      </c>
+      <c r="O86" t="s">
+        <v>11</v>
+      </c>
+      <c r="P86" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>11</v>
+      </c>
+      <c r="R86" t="s">
+        <v>11</v>
+      </c>
+      <c r="S86" t="b">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>9869.0254278273824</v>
+      </c>
+      <c r="U86" t="b">
+        <v>1</v>
+      </c>
+      <c r="V86">
+        <v>3</v>
+      </c>
+      <c r="W86">
+        <v>8</v>
+      </c>
+      <c r="X86">
+        <v>1</v>
+      </c>
+      <c r="Y86">
+        <v>86.191207885742188</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>117</v>
+      </c>
+      <c r="B87" t="s">
+        <v>109</v>
+      </c>
+      <c r="C87" t="s">
+        <v>62</v>
+      </c>
+      <c r="D87" t="s">
+        <v>45</v>
+      </c>
+      <c r="E87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" t="s">
+        <v>47</v>
+      </c>
+      <c r="G87" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" t="s">
+        <v>11</v>
+      </c>
+      <c r="I87" t="s">
+        <v>11</v>
+      </c>
+      <c r="J87">
+        <v>14.440381050109863</v>
+      </c>
+      <c r="K87">
+        <v>14.576918601989746</v>
+      </c>
+      <c r="L87">
+        <v>0.12103687971830368</v>
+      </c>
+      <c r="M87" t="s">
+        <v>11</v>
+      </c>
+      <c r="N87" t="s">
+        <v>11</v>
+      </c>
+      <c r="O87" t="s">
+        <v>11</v>
+      </c>
+      <c r="P87" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>11</v>
+      </c>
+      <c r="R87" t="s">
+        <v>11</v>
+      </c>
+      <c r="S87" t="b">
+        <v>1</v>
+      </c>
+      <c r="T87">
+        <v>9869.0254278273824</v>
+      </c>
+      <c r="U87" t="b">
+        <v>1</v>
+      </c>
+      <c r="V87">
+        <v>3</v>
+      </c>
+      <c r="W87">
         <v>6</v>
       </c>
-      <c r="X84">
-        <v>1</v>
-      </c>
-      <c r="Y84">
+      <c r="X87">
+        <v>1</v>
+      </c>
+      <c r="Y87">
         <v>86.191207885742188</v>
       </c>
-      <c r="Z84" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA84" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB84" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC84" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="Z87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC87" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>118</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>120</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B90" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>121</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>123</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B92" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>